<commit_message>
add interface for power analysis
</commit_message>
<xml_diff>
--- a/PlantAnalysis/result30210.xlsx
+++ b/PlantAnalysis/result30210.xlsx
@@ -135,37 +135,37 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2.36483</t>
+          <t>2.40371</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>19.3852</t>
+          <t>3.46816</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2.2846363</t>
+          <t>2.3167598</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>3.6108463</t>
+          <t>3.4968402</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2.781965</t>
+          <t>2.75929</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>3.1135175</t>
+          <t>3.05431</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0.3315525</t>
+          <t>0.2950201</t>
         </is>
       </c>
     </row>
@@ -177,37 +177,37 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2.52964</t>
+          <t>2.84243</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>4.71718</t>
+          <t>3.71883</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2.734895</t>
+          <t>2.77497</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>3.809375</t>
+          <t>3.7529697</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>3.137825</t>
+          <t>3.14172</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>3.406445</t>
+          <t>3.38622</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>0.26862</t>
+          <t>0.24449992</t>
         </is>
       </c>
     </row>
@@ -219,37 +219,37 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>3.153</t>
+          <t>3.23279</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>5.60875</t>
+          <t>4.03014</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>3.1838527</t>
+          <t>3.1867611</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>4.090552</t>
+          <t>4.085471</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>3.523865</t>
+          <t>3.5237775</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>3.7505398</t>
+          <t>3.748455</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>0.2266748</t>
+          <t>0.22467756</t>
         </is>
       </c>
     </row>
@@ -266,17 +266,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>7.83407</t>
+          <t>4.35584</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>3.6003098</t>
+          <t>3.62782</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>4.44311</t>
+          <t>4.3972597</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -286,12 +286,12 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>4.12706</t>
+          <t>4.10872</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>0.21070004</t>
+          <t>0.19235992</t>
         </is>
       </c>
     </row>
@@ -303,27 +303,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3.88184</t>
+          <t>4.0022</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>4.95741</t>
+          <t>4.78218</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>3.8766043</t>
+          <t>3.8917284</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>4.803673</t>
+          <t>4.7945986</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>4.224255</t>
+          <t>4.2303047</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -333,7 +333,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>0.23176718</t>
+          <t>0.22571754</t>
         </is>
       </c>
     </row>
@@ -345,37 +345,37 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>3.98932</t>
+          <t>4.20298</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>6.85805</t>
+          <t>4.91426</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>4.13998</t>
+          <t>4.1754317</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>4.98574</t>
+          <t>4.9193015</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>4.45714</t>
+          <t>4.454383</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>4.66858</t>
+          <t>4.6403503</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>0.21144009</t>
+          <t>0.18596745</t>
         </is>
       </c>
     </row>
@@ -387,22 +387,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>4.25361</t>
+          <t>4.41224</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>18.0598</t>
+          <t>5.12772</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>4.316186</t>
+          <t>4.321109</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>5.220237</t>
+          <t>5.2120314</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -412,12 +412,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>4.8812175</t>
+          <t>4.8779354</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>0.2260127</t>
+          <t>0.22273064</t>
         </is>
       </c>
     </row>
@@ -429,37 +429,37 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>4.67739</t>
+          <t>4.7026</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>5.44308</t>
+          <t>5.38515</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>4.5635695</t>
+          <t>4.5760746</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>5.4069304</t>
+          <t>5.3925953</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>4.87983</t>
+          <t>4.88227</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>5.09067</t>
+          <t>5.0864</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>0.21084023</t>
+          <t>0.20413017</t>
         </is>
       </c>
     </row>
@@ -471,37 +471,37 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>4.78024</t>
+          <t>4.95018</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>5.87793</t>
+          <t>5.45509</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>4.4675045</t>
+          <t>4.8851676</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>6.724186</t>
+          <t>5.530088</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>5.31376</t>
+          <t>5.1270127</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>5.87793</t>
+          <t>5.288243</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>0.56417036</t>
+          <t>0.16123009</t>
         </is>
       </c>
     </row>
@@ -513,37 +513,37 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>4.96568</t>
+          <t>5.05881</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>13.4014</t>
+          <t>5.73699</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>4.941633</t>
+          <t>4.951241</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>5.821192</t>
+          <t>5.7920117</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>5.2714677</t>
+          <t>5.26653</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>5.4913573</t>
+          <t>5.4767227</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>0.21988964</t>
+          <t>0.21019268</t>
         </is>
       </c>
     </row>
@@ -555,37 +555,37 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>5.03852</t>
+          <t>5.13802</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>15.6168</t>
+          <t>5.85495</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>5.1307893</t>
+          <t>5.109502</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>5.856631</t>
+          <t>5.8925753</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>5.40298</t>
+          <t>5.4031544</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>5.58444</t>
+          <t>5.5989227</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>0.18146038</t>
+          <t>0.19576836</t>
         </is>
       </c>
     </row>
@@ -597,37 +597,37 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>5.26289</t>
+          <t>5.27831</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>6.21475</t>
+          <t>5.9321</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>5.27709</t>
+          <t>5.275916</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>5.96525</t>
+          <t>5.944646</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>5.53515</t>
+          <t>5.52669</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>5.70719</t>
+          <t>5.6938725</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>0.17203999</t>
+          <t>0.16718245</t>
         </is>
       </c>
     </row>
@@ -644,17 +644,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>6.31977</t>
+          <t>6.25737</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>5.312125</t>
+          <t>5.3244247</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>6.328885</t>
+          <t>6.308386</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -664,12 +664,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>5.9476</t>
+          <t>5.9394</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>0.25418997</t>
+          <t>0.24599028</t>
         </is>
       </c>
     </row>
@@ -691,27 +691,27 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>5.514325</t>
+          <t>5.5327597</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>6.304097</t>
+          <t>6.29432</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>5.8104897</t>
+          <t>5.818345</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>6.0079327</t>
+          <t>6.008735</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>0.19744301</t>
+          <t>0.19039011</t>
         </is>
       </c>
     </row>
@@ -723,37 +723,37 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>5.67417</t>
+          <t>5.7483</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>6.77122</t>
+          <t>6.39308</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>5.6659555</t>
+          <t>5.696583</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>6.4558344</t>
+          <t>6.4042225</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>5.96216</t>
+          <t>5.9619474</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>6.15963</t>
+          <t>6.1388574</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>0.19746971</t>
+          <t>0.17690992</t>
         </is>
       </c>
     </row>
@@ -770,32 +770,32 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>6.56427</t>
+          <t>6.49596</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>5.793624</t>
+          <t>5.7666445</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>6.5645456</t>
+          <t>6.573886</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>6.08272</t>
+          <t>6.06936</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>6.27545</t>
+          <t>6.27117</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>0.19273043</t>
+          <t>0.20181036</t>
         </is>
       </c>
     </row>
@@ -812,17 +812,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>6.82468</t>
+          <t>6.61804</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>5.883135</t>
+          <t>5.89896</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>6.702135</t>
+          <t>6.6757603</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -832,12 +832,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>6.39501</t>
+          <t>6.38446</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>0.20475006</t>
+          <t>0.19420004</t>
         </is>
       </c>
     </row>
@@ -849,37 +849,37 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>6.05282</t>
+          <t>6.10651</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>6.80508</t>
+          <t>6.73278</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>6.056555</t>
+          <t>6.071066</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>6.748356</t>
+          <t>6.743269</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>6.31598</t>
+          <t>6.323142</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>6.48893</t>
+          <t>6.491193</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>0.17295027</t>
+          <t>0.16805077</t>
         </is>
       </c>
     </row>
@@ -891,37 +891,37 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>6.20847</t>
+          <t>6.31666</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>6.90125</t>
+          <t>6.78438</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>6.2180986</t>
+          <t>6.237776</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>6.808936</t>
+          <t>6.794134</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>6.439663</t>
+          <t>6.44641</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>6.5873723</t>
+          <t>6.5855</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>0.14770937</t>
+          <t>0.13908958</t>
         </is>
       </c>
     </row>
@@ -933,37 +933,37 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>6.3265</t>
+          <t>6.39952</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>7.23578</t>
+          <t>6.82628</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>6.3440304</t>
+          <t>6.389537</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>6.89575</t>
+          <t>6.828418</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>6.5509253</t>
+          <t>6.554117</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>6.688855</t>
+          <t>6.6638374</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>0.13792992</t>
+          <t>0.10972023</t>
         </is>
       </c>
     </row>
@@ -980,17 +980,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>7.1613</t>
+          <t>7.00331</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>6.336893</t>
+          <t>6.345589</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>7.140772</t>
+          <t>7.1262784</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1000,12 +1000,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>6.8393173</t>
+          <t>6.83352</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>0.2009697</t>
+          <t>0.19517231</t>
         </is>
       </c>
     </row>
@@ -1022,32 +1022,32 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>7.71646</t>
+          <t>7.22031</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>6.4598565</t>
+          <t>6.4801593</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>7.3033586</t>
+          <t>7.26448</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>6.77617</t>
+          <t>6.7742796</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>6.9870453</t>
+          <t>6.97036</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>0.21087551</t>
+          <t>0.19608021</t>
         </is>
       </c>
     </row>
@@ -1064,7 +1064,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>8.31837</t>
+          <t>7.27854</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1106,32 +1106,32 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>7.58043</t>
+          <t>7.44421</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>6.5672827</t>
+          <t>6.6208544</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>7.5817423</t>
+          <t>7.4869833</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>6.947705</t>
+          <t>6.9456525</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>7.2013197</t>
+          <t>7.1621847</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>0.2536149</t>
+          <t>0.21653223</t>
         </is>
       </c>
     </row>
@@ -1148,32 +1148,32 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>7.83485</t>
+          <t>7.49063</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>6.698335</t>
+          <t>6.7360973</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>7.705095</t>
+          <t>7.639717</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>7.07587</t>
+          <t>7.074955</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>7.32756</t>
+          <t>7.30086</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>0.2516899</t>
+          <t>0.22590494</t>
         </is>
       </c>
     </row>
@@ -1190,32 +1190,32 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>8.08716</t>
+          <t>7.71829</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>6.7022743</t>
+          <t>6.699946</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>7.862955</t>
+          <t>7.855864</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>7.13753</t>
+          <t>7.133415</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>7.4277</t>
+          <t>7.4223948</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>0.2901702</t>
+          <t>0.28897953</t>
         </is>
       </c>
     </row>
@@ -1227,37 +1227,37 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>7.00823</t>
+          <t>7.12946</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>7.92957</t>
+          <t>7.77535</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>6.952085</t>
+          <t>6.9847307</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>7.863725</t>
+          <t>7.8039293</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>7.29395</t>
+          <t>7.29193</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>7.52186</t>
+          <t>7.49673</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>0.22791004</t>
+          <t>0.20479965</t>
         </is>
       </c>
     </row>
@@ -1274,32 +1274,32 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>8.26543</t>
+          <t>7.89407</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>6.939507</t>
+          <t>7.008897</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>8.044407</t>
+          <t>7.9271784</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>7.3538446</t>
+          <t>7.3532524</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>7.6300697</t>
+          <t>7.582823</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>0.2762251</t>
+          <t>0.22957039</t>
         </is>
       </c>
     </row>
@@ -1316,32 +1316,32 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>8.3008</t>
+          <t>8.11983</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>7.0483594</t>
+          <t>7.0674853</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>8.10392</t>
+          <t>8.130405</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>7.444195</t>
+          <t>7.46608</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>7.708085</t>
+          <t>7.73181</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>0.26389027</t>
+          <t>0.2657299</t>
         </is>
       </c>
     </row>
@@ -1358,7 +1358,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>8.27029</t>
+          <t>8.16639</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1395,22 +1395,22 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>7.33433</t>
+          <t>7.49983</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>8.57931</t>
+          <t>8.17683</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>7.327257</t>
+          <t>7.357216</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>8.349598</t>
+          <t>8.299665</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1420,12 +1420,12 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>7.96622</t>
+          <t>7.946247</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>0.2555852</t>
+          <t>0.23561239</t>
         </is>
       </c>
     </row>
@@ -1442,7 +1442,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>8.70134</t>
+          <t>8.48147</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1484,32 +1484,32 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>9.86694</t>
+          <t>8.64726</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>7.303712</t>
+          <t>7.3051987</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>8.713973</t>
+          <t>8.711922</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>7.83256</t>
+          <t>7.83272</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>8.185125</t>
+          <t>8.184401</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>0.3525653</t>
+          <t>0.35168076</t>
         </is>
       </c>
     </row>
@@ -1526,32 +1526,32 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>9.78803</t>
+          <t>8.80308</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>7.5057106</t>
+          <t>7.5488973</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>8.899517</t>
+          <t>8.814373</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>8.028388</t>
+          <t>8.023451</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>8.37684</t>
+          <t>8.33982</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>0.3484516</t>
+          <t>0.31636906</t>
         </is>
       </c>
     </row>
@@ -1568,32 +1568,32 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>9.68111</t>
+          <t>9.05567</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>7.500586</t>
+          <t>7.500131</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>9.152224</t>
+          <t>9.085409</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>8.11995</t>
+          <t>8.09461</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>8.53286</t>
+          <t>8.49093</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>0.4129095</t>
+          <t>0.3963194</t>
         </is>
       </c>
     </row>
@@ -1605,37 +1605,37 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>7.94558</t>
+          <t>8.03066</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>9.72107</t>
+          <t>9.05569</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>7.564077</t>
+          <t>7.6779304</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>9.272486</t>
+          <t>9.068918</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>8.20473</t>
+          <t>8.199551</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>8.631832</t>
+          <t>8.5472975</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>0.4271021</t>
+          <t>0.34774685</t>
         </is>
       </c>
     </row>
@@ -1652,32 +1652,32 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>9.7829</t>
+          <t>9.52215</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>7.4295144</t>
+          <t>7.4450426</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>9.8077755</t>
+          <t>9.780408</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>8.3213625</t>
+          <t>8.320805</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>8.915928</t>
+          <t>8.904646</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>0.5945654</t>
+          <t>0.5838413</t>
         </is>
       </c>
     </row>
@@ -1694,32 +1694,32 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>11.0892</t>
+          <t>9.42961</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>7.597285</t>
+          <t>7.78509</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>9.750036</t>
+          <t>9.43685</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>8.404567</t>
+          <t>8.4045</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>8.942755</t>
+          <t>8.81744</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>0.538188</t>
+          <t>0.41294003</t>
         </is>
       </c>
     </row>
@@ -1736,32 +1736,32 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>10.6279</t>
+          <t>9.50515</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>7.883671</t>
+          <t>7.840236</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>9.505909</t>
+          <t>9.529839</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>8.49201</t>
+          <t>8.473837</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>8.89757</t>
+          <t>8.896237</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>0.40555954</t>
+          <t>0.42240047</t>
         </is>
       </c>
     </row>
@@ -1778,32 +1778,32 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>10.2</t>
+          <t>9.71923</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>7.800561</t>
+          <t>7.898691</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>9.933885</t>
+          <t>9.741129</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>8.600557</t>
+          <t>8.589605</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>9.133888</t>
+          <t>9.050215</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>0.5333309</t>
+          <t>0.46060944</t>
         </is>
       </c>
     </row>
@@ -1820,32 +1820,32 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>10.9401</t>
+          <t>9.95315</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>7.8557777</t>
+          <t>7.8910246</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>10.303898</t>
+          <t>10.234546</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>8.773823</t>
+          <t>8.769845</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>9.385853</t>
+          <t>9.355725</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>0.61203</t>
+          <t>0.5858803</t>
         </is>
       </c>
     </row>
@@ -1862,32 +1862,32 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>11.0958</t>
+          <t>10.1859</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>7.907039</t>
+          <t>7.894397</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>10.267288</t>
+          <t>10.188579</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>8.792132</t>
+          <t>8.754715</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>9.3821945</t>
+          <t>9.32826</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>0.59006214</t>
+          <t>0.57354546</t>
         </is>
       </c>
     </row>
@@ -1904,32 +1904,32 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>10.7903</t>
+          <t>10.4996</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>7.802656</t>
+          <t>7.824564</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>10.750013</t>
+          <t>10.699015</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>8.907915</t>
+          <t>8.902483</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>9.644754</t>
+          <t>9.621096</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>0.7368393</t>
+          <t>0.7186127</t>
         </is>
       </c>
     </row>
@@ -1946,32 +1946,32 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>12.3642</t>
+          <t>10.2293</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>8.117272</t>
+          <t>8.282532</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>10.665681</t>
+          <t>10.257992</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>9.072926</t>
+          <t>9.02333</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>9.710028</t>
+          <t>9.517195</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>0.6371021</t>
+          <t>0.493865</t>
         </is>
       </c>
     </row>
@@ -1988,32 +1988,32 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>13.6263</t>
+          <t>10.8424</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>7.70221</t>
+          <t>7.892858</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>11.216038</t>
+          <t>10.868998</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>9.019896</t>
+          <t>9.00891</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>9.898353</t>
+          <t>9.752945</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>0.87845707</t>
+          <t>0.74403477</t>
         </is>
       </c>
     </row>
@@ -2025,37 +2025,37 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>8.44181</t>
+          <t>8.59828</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>12.5301</t>
+          <t>11.0772</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>7.797049</t>
+          <t>8.071751</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>11.377611</t>
+          <t>10.9339905</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>9.13976</t>
+          <t>9.14509</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>10.034901</t>
+          <t>9.86065</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>0.89514065</t>
+          <t>0.71555996</t>
         </is>
       </c>
     </row>
@@ -2072,32 +2072,32 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>15.3671</t>
+          <t>11.9792</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>7.779388</t>
+          <t>7.8120813</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>12.065647</t>
+          <t>11.987031</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>9.386735</t>
+          <t>9.377687</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>10.4583</t>
+          <t>10.421425</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>1.0715647</t>
+          <t>1.0437374</t>
         </is>
       </c>
     </row>
@@ -2109,37 +2109,37 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>8.49133</t>
+          <t>8.53711</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>14.7556</t>
+          <t>12.5202</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>7.203087</t>
+          <t>7.312056</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>13.172829</t>
+          <t>13.010767</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>9.44174</t>
+          <t>9.449073</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>10.9341755</t>
+          <t>10.873751</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>1.4924355</t>
+          <t>1.4246778</t>
         </is>
       </c>
     </row>
@@ -2156,32 +2156,32 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>13.4801</t>
+          <t>12.6986</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>7.491337</t>
+          <t>7.5930495</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>12.866398</t>
+          <t>12.727972</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>9.506985</t>
+          <t>9.518645</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>10.85075</t>
+          <t>10.802376</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>1.3437653</t>
+          <t>1.2837305</t>
         </is>
       </c>
     </row>
@@ -2198,32 +2198,32 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>15.0575</t>
+          <t>12.8377</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>7.6817074</t>
+          <t>7.987313</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>13.437735</t>
+          <t>12.789532</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>9.840218</t>
+          <t>9.788145</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>11.279224</t>
+          <t>10.9887</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>1.4390068</t>
+          <t>1.2005548</t>
         </is>
       </c>
     </row>
@@ -2240,32 +2240,32 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15.648</t>
+          <t>14.137</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>7.109164</t>
+          <t>7.1573997</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>14.440341</t>
+          <t>14.344881</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>9.8583555</t>
+          <t>9.852705</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>11.69115</t>
+          <t>11.649575</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>1.8327942</t>
+          <t>1.7968702</t>
         </is>
       </c>
     </row>
@@ -2282,32 +2282,32 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>24.4979</t>
+          <t>15.3053</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>7.213801</t>
+          <t>7.0141625</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>15.037199</t>
+          <t>15.380262</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>10.147575</t>
+          <t>10.15145</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>12.103425</t>
+          <t>12.242975</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>1.9558496</t>
+          <t>2.091525</t>
         </is>
       </c>
     </row>
@@ -2329,27 +2329,27 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>6.4547253</t>
+          <t>6.6149626</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>17.106924</t>
+          <t>16.854664</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>10.4493</t>
+          <t>10.45485</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>13.1123495</t>
+          <t>13.014775</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>2.6630497</t>
+          <t>2.559925</t>
         </is>
       </c>
     </row>
@@ -2366,32 +2366,32 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>20.4419</t>
+          <t>16.3535</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>6.7966237</t>
+          <t>6.908149</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>17.880825</t>
+          <t>17.670952</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>10.953199</t>
+          <t>10.9442</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>13.72425</t>
+          <t>13.6349</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>2.7710505</t>
+          <t>2.6907005</t>
         </is>
       </c>
     </row>
@@ -2413,27 +2413,27 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>6.546063</t>
+          <t>6.4063005</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>18.914162</t>
+          <t>18.955898</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>11.1841</t>
+          <t>11.1124</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>14.276125</t>
+          <t>14.2498</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>3.0920248</t>
+          <t>3.1373997</t>
         </is>
       </c>
     </row>
@@ -2455,27 +2455,27 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>6.8070126</t>
+          <t>6.77965</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>18.889112</t>
+          <t>18.98725</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>11.3378</t>
+          <t>11.3575</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>14.358325</t>
+          <t>14.4094</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>3.020525</t>
+          <t>3.0519</t>
         </is>
       </c>
     </row>
@@ -2492,22 +2492,22 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>20.528</t>
+          <t>18.5427</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>6.0423512</t>
+          <t>6.151225</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>20.43575</t>
+          <t>20.370426</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>11.439876</t>
+          <t>11.483425</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
@@ -2517,7 +2517,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>3.5983496</t>
+          <t>3.5548</t>
         </is>
       </c>
     </row>
@@ -2539,27 +2539,27 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>7.0654774</t>
+          <t>7.059612</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>20.043673</t>
+          <t>20.047714</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>11.932301</t>
+          <t>11.93015</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>15.176849</t>
+          <t>15.1771755</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>3.2445488</t>
+          <t>3.2470255</t>
         </is>
       </c>
     </row>
@@ -2576,32 +2576,32 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>25.3825</t>
+          <t>21.9361</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>6.184638</t>
+          <t>6.202902</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>22.168137</t>
+          <t>22.143698</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>12.17845</t>
+          <t>12.1807</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>16.174324</t>
+          <t>16.1659</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>3.9958744</t>
+          <t>3.985199</t>
         </is>
       </c>
     </row>
@@ -2618,32 +2618,32 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>23.9343</t>
+          <t>20.9462</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>7.249828</t>
+          <t>7.3567</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>22.519821</t>
+          <t>22.3559</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>12.976075</t>
+          <t>12.9814</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>16.793573</t>
+          <t>16.7312</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>3.8174982</t>
+          <t>3.7497997</t>
         </is>
       </c>
     </row>
@@ -2665,27 +2665,27 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>6.7453985</t>
+          <t>6.8296766</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>24.794205</t>
+          <t>24.689075</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>13.5137005</t>
+          <t>13.526951</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>18.025902</t>
+          <t>17.9918</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>4.5122013</t>
+          <t>4.4648495</t>
         </is>
       </c>
     </row>
@@ -2739,37 +2739,37 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>-4.37398</t>
+          <t>-3.75988</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>-1.2715</t>
+          <t>-1.46988</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>-4.37398</t>
+          <t>-3.75988</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>-1.4163802</t>
+          <t>-1.44486</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>-1.79808</t>
+          <t>-1.79421</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>-1.6454</t>
+          <t>-1.65447</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>0.15267992</t>
+          <t>0.13973999</t>
         </is>
       </c>
     </row>
@@ -2786,7 +2786,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>-1.29548</t>
+          <t>-1.40992</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2796,22 +2796,22 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>-1.3659301</t>
+          <t>-1.3761761</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>-1.86383</t>
+          <t>-1.85927</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>-1.66467</t>
+          <t>-1.6660324</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>0.19915998</t>
+          <t>0.19323754</t>
         </is>
       </c>
     </row>
@@ -2828,7 +2828,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>-1.29467</t>
+          <t>-1.30932</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2838,22 +2838,22 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>-1.3019687</t>
+          <t>-1.30691</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>-1.9451874</t>
+          <t>-1.95001</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>-1.6879</t>
+          <t>-1.69277</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>0.2572875</t>
+          <t>0.25723994</t>
         </is>
       </c>
     </row>
@@ -2880,22 +2880,22 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>-1.1177752</t>
+          <t>-1.1361952</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>-2.084775</t>
+          <t>-2.0681448</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>-1.697975</t>
+          <t>-1.695365</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>0.38679993</t>
+          <t>0.37277985</t>
         </is>
       </c>
     </row>
@@ -2912,7 +2912,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>7.51938</t>
+          <t>0.17956</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2922,22 +2922,22 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>0.34893012</t>
+          <t>0.4066676</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>-3.09482</t>
+          <t>-3.1500576</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>-1.71732</t>
+          <t>-1.7273675</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>1.3775</t>
+          <t>1.42269</t>
         </is>
       </c>
     </row>
@@ -2954,7 +2954,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>39.4671</t>
+          <t>30.949</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2964,22 +2964,22 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>32.73163</t>
+          <t>31.285885</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>-2.96192</t>
+          <t>-2.9640076</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>11.3155</t>
+          <t>10.7359495</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>14.27742</t>
+          <t>13.699957</t>
         </is>
       </c>
     </row>
@@ -3006,22 +3006,22 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>86.46605</t>
+          <t>87.46965</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>14.299925</t>
+          <t>13.6304</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>43.166374</t>
+          <t>43.1661</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>28.86645</t>
+          <t>29.5357</t>
         </is>
       </c>
     </row>
@@ -3038,7 +3038,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>114.33</t>
+          <t>99.1296</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -3048,22 +3048,22 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>107.9281</t>
+          <t>108.70552</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>55.981598</t>
+          <t>56.0224</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>76.7602</t>
+          <t>77.09565</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>20.778603</t>
+          <t>21.07325</t>
         </is>
       </c>
     </row>
@@ -3080,7 +3080,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>172.664</t>
+          <t>157.922</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -3090,22 +3090,22 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>159.88394</t>
+          <t>158.9335</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>94.6207</t>
+          <t>94.2635</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>120.726</t>
+          <t>120.1315</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>26.1053</t>
+          <t>25.868004</t>
         </is>
       </c>
     </row>
@@ -3117,37 +3117,37 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>-7.70337</t>
+          <t>-5.05757</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>227.89</t>
+          <t>200.541</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>-7.70337</t>
+          <t>-5.05757</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>232.47797</t>
+          <t>226.44897</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>138.90425</t>
+          <t>138.634</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>176.33374</t>
+          <t>173.76</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>37.42949</t>
+          <t>35.12599</t>
         </is>
       </c>
     </row>
@@ -3159,7 +3159,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>-7.87226</t>
+          <t>-3.94331</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3169,27 +3169,27 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>-7.87226</t>
+          <t>-3.94331</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>315.15594</t>
+          <t>329.7895</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>202.00601</t>
+          <t>199.067</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>247.26599</t>
+          <t>251.356</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>45.25998</t>
+          <t>52.289</t>
         </is>
       </c>
     </row>
@@ -3216,22 +3216,22 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>461.11517</t>
+          <t>422.32397</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>203.952</t>
+          <t>276.22275</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>306.81726</t>
+          <t>334.66324</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>102.865265</t>
+          <t>58.44049</t>
         </is>
       </c>
     </row>
@@ -3243,7 +3243,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>-7.57737</t>
+          <t>301.93</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3253,27 +3253,27 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>-7.57737</t>
+          <t>301.93</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>529.3258</t>
+          <t>520.7577</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>372.70276</t>
+          <t>373.52698</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>435.352</t>
+          <t>432.41925</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>62.64923</t>
+          <t>58.892273</t>
         </is>
       </c>
     </row>
@@ -3285,7 +3285,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>-7.75892</t>
+          <t>418.671</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3295,27 +3295,27 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>-7.75892</t>
+          <t>418.671</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>642.5174</t>
+          <t>641.00275</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>486.21674</t>
+          <t>488.11526</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>548.737</t>
+          <t>549.27026</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>62.520264</t>
+          <t>61.155</t>
         </is>
       </c>
     </row>
@@ -3332,7 +3332,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>755.832</t>
+          <t>754.552</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -3342,22 +3342,22 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>790.2845</t>
+          <t>785.21136</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>598.527</t>
+          <t>598.1795</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>675.23</t>
+          <t>672.99225</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>76.703</t>
+          <t>74.812744</t>
         </is>
       </c>
     </row>
@@ -3369,37 +3369,37 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>585.214</t>
+          <t>647.135</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>883.783</t>
+          <t>873.713</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>585.214</t>
+          <t>647.135</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>901.0869</t>
+          <t>898.16455</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>717.45703</t>
+          <t>719.282</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>790.909</t>
+          <t>790.835</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>73.451965</t>
+          <t>71.55304</t>
         </is>
       </c>
     </row>
@@ -3411,37 +3411,37 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>-10.3014</t>
+          <t>704.723</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>1187.14</t>
+          <t>1049.92</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>-10.3014</t>
+          <t>704.723</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>1057.0068</t>
+          <t>1051.3701</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>832.7388</t>
+          <t>831.1</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>922.446</t>
+          <t>919.208</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>89.707214</t>
+          <t>88.10803</t>
         </is>
       </c>
     </row>
@@ -3453,37 +3453,37 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>784.246</t>
+          <t>801.249</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>1222.24</t>
+          <t>1209.25</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>784.246</t>
+          <t>801.249</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>1218.3223</t>
+          <t>1214.074</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>932.91003</t>
+          <t>935.5465</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>1047.075</t>
+          <t>1046.9575</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>114.16492</t>
+          <t>111.41101</t>
         </is>
       </c>
     </row>
@@ -3510,22 +3510,22 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>1377.0577</t>
+          <t>1378.575</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>1025.845</t>
+          <t>1024.65</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>1166.3301</t>
+          <t>1166.22</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>140.4851</t>
+          <t>141.56995</t>
         </is>
       </c>
     </row>
@@ -3537,7 +3537,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>920.963</t>
+          <t>921.407</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3547,27 +3547,27 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>920.963</t>
+          <t>921.407</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>1489.7311</t>
+          <t>1482.894</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>1117.5625</t>
+          <t>1120.5249</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>1266.4299</t>
+          <t>1265.4725</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>148.86743</t>
+          <t>144.94763</t>
         </is>
       </c>
     </row>
@@ -3579,7 +3579,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>1003.45</t>
+          <t>1032.17</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3589,27 +3589,27 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>1003.45</t>
+          <t>1032.17</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>1538.335</t>
+          <t>1534.135</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>1192.0975</t>
+          <t>1198.21</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>1330.5925</t>
+          <t>1332.58</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>138.495</t>
+          <t>134.37</t>
         </is>
       </c>
     </row>
@@ -3621,7 +3621,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>1069.15</t>
+          <t>1109.16</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3631,17 +3631,17 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>1069.15</t>
+          <t>1109.16</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>1618.0652</t>
+          <t>1617.5625</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>1244.4275</t>
+          <t>1244.7626</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
@@ -3651,7 +3651,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>149.45508</t>
+          <t>149.12</t>
         </is>
       </c>
     </row>
@@ -3663,7 +3663,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>1116.73</t>
+          <t>1150.08</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3673,17 +3673,17 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>1116.73</t>
+          <t>1150.08</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>1630.0302</t>
+          <t>1620.1001</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>1285.48</t>
+          <t>1292.1</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
@@ -3693,7 +3693,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>137.82007</t>
+          <t>131.20007</t>
         </is>
       </c>
     </row>
@@ -3705,7 +3705,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>-9.11775</t>
+          <t>1150.49</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3715,12 +3715,12 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>-9.11775</t>
+          <t>1150.49</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>1668.8413</t>
+          <t>1661.6849</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -3730,12 +3730,12 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>1439.8251</t>
+          <t>1436.9625</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>152.67749</t>
+          <t>149.81494</t>
         </is>
       </c>
     </row>
@@ -3762,22 +3762,22 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>1661.005</t>
+          <t>1657.21</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>1319.6799</t>
+          <t>1319.71</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>1456.21</t>
+          <t>1454.71</t>
         </is>
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>136.53003</t>
+          <t>135.0</t>
         </is>
       </c>
     </row>
@@ -3804,22 +3804,22 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>1665.7211</t>
+          <t>1664.251</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>1340.4275</t>
+          <t>1341.195</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>1470.5449</t>
+          <t>1470.4174</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>130.11743</t>
+          <t>129.22241</t>
         </is>
       </c>
     </row>
@@ -3831,7 +3831,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>1232.73</t>
+          <t>1261.55</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3841,27 +3841,27 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>1232.73</t>
+          <t>1261.55</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>1645.6736</t>
+          <t>1641.1511</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>1346.43</t>
+          <t>1350.2576</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>1466.1274</t>
+          <t>1466.615</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>119.69739</t>
+          <t>116.35742</t>
         </is>
       </c>
     </row>
@@ -3888,22 +3888,22 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>1658.2349</t>
+          <t>1660.3088</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>1334.4974</t>
+          <t>1333.09</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>1463.9924</t>
+          <t>1463.9775</t>
         </is>
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>129.495</t>
+          <t>130.88757</t>
         </is>
       </c>
     </row>
@@ -3930,12 +3930,12 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>1657.2588</t>
+          <t>1656.4714</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>1363.04</t>
+          <t>1363.565</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
@@ -3945,7 +3945,7 @@
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>117.6875</t>
+          <t>117.1626</t>
         </is>
       </c>
     </row>
@@ -3972,12 +3972,12 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>1640.416</t>
+          <t>1638.211</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>1374.285</t>
+          <t>1375.755</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
@@ -3987,7 +3987,7 @@
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>106.45239</t>
+          <t>104.98242</t>
         </is>
       </c>
     </row>
@@ -4014,7 +4014,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>1626.0059</t>
+          <t>1620.1125</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -4024,12 +4024,12 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>1477.0299</t>
+          <t>1474.6726</t>
         </is>
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>99.31726</t>
+          <t>96.95996</t>
         </is>
       </c>
     </row>
@@ -4041,7 +4041,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>-7.94037</t>
+          <t>1327.44</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -4051,27 +4051,27 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>-7.94037</t>
+          <t>1327.44</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>1609.4</t>
+          <t>1609.6626</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>1413.7</t>
+          <t>1410.2</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>1491.98</t>
+          <t>1489.985</t>
         </is>
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>78.28003</t>
+          <t>79.785034</t>
         </is>
       </c>
     </row>
@@ -4083,7 +4083,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>-8.27627</t>
+          <t>1311.47</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -4093,27 +4093,27 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>-8.27627</t>
+          <t>1311.47</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>1584.7277</t>
+          <t>1581.0122</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>1423.615</t>
+          <t>1426.3501</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>1488.06</t>
+          <t>1488.215</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>64.44507</t>
+          <t>61.86487</t>
         </is>
       </c>
     </row>
@@ -4140,22 +4140,22 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>1580.939</t>
+          <t>1582.2151</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>1438.9824</t>
+          <t>1437.94</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>1495.765</t>
+          <t>1495.65</t>
         </is>
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>56.782593</t>
+          <t>57.710083</t>
         </is>
       </c>
     </row>
@@ -4182,22 +4182,22 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>1594.9424</t>
+          <t>1600.3947</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>1437.88</t>
+          <t>1434.1825</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>1500.705</t>
+          <t>1500.6674</t>
         </is>
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>62.82495</t>
+          <t>66.48486</t>
         </is>
       </c>
     </row>
@@ -4224,12 +4224,12 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>1586.1387</t>
+          <t>1578.9426</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>1438.27</t>
+          <t>1443.0674</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
@@ -4239,7 +4239,7 @@
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>59.14746</t>
+          <t>54.350098</t>
         </is>
       </c>
     </row>
@@ -4293,7 +4293,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>-8.18434</t>
+          <t>-8.10152</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -4303,27 +4303,27 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>-8.18434</t>
+          <t>-8.10152</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>1594.0735</t>
+          <t>1564.9897</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>1439.305</t>
+          <t>1458.7151</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>1501.2124</t>
+          <t>1501.225</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>61.90735</t>
+          <t>42.509888</t>
         </is>
       </c>
     </row>
@@ -4350,22 +4350,22 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>1565.3524</t>
+          <t>1562.355</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>1459.44</t>
+          <t>1461.33</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>1501.8049</t>
+          <t>1501.74</t>
         </is>
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>42.36499</t>
+          <t>40.410034</t>
         </is>
       </c>
     </row>
@@ -4392,22 +4392,22 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>3763.4307</t>
+          <t>3763.2778</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>-7.4035854</t>
+          <t>-7.38527</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>1500.93</t>
+          <t>1500.88</t>
         </is>
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>1508.3336</t>
+          <t>1508.2653</t>
         </is>
       </c>
     </row>
@@ -4419,7 +4419,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>-7.47133</t>
+          <t>1466.42</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -4429,27 +4429,27 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>-7.47133</t>
+          <t>1466.42</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>1546.1549</t>
+          <t>1512.7101</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>1469.1426</t>
+          <t>1492.01</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>1499.9475</t>
+          <t>1500.29</t>
         </is>
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>30.804932</t>
+          <t>8.280029</t>
         </is>
       </c>
     </row>
@@ -4476,22 +4476,22 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>3739.7446</t>
+          <t>3740.5977</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>-3.2714</t>
+          <t>-1.8108575</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>1493.935</t>
+          <t>1495.1525</t>
         </is>
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>1497.2064</t>
+          <t>1496.9634</t>
         </is>
       </c>
     </row>
@@ -4503,37 +4503,37 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>-8.18848</t>
+          <t>-7.59543</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>1479.62</t>
+          <t>-1.83502</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>-8.18848</t>
+          <t>-7.59543</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>2766.1357</t>
+          <t>1.9949852</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>-4.69245</t>
+          <t>-4.59669</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>1103.6388</t>
+          <t>-1.96002</t>
         </is>
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>1108.3313</t>
+          <t>2.63667</t>
         </is>
       </c>
     </row>
@@ -4587,22 +4587,22 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>-4.81724</t>
+          <t>-4.74352</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>1496.93</t>
+          <t>-1.94992</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>-4.81724</t>
+          <t>-4.74352</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>3709.4824</t>
+          <t>2.2155423</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -4612,94 +4612,52 @@
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>1480.95</t>
+          <t>-1.9568576</t>
         </is>
       </c>
       <c r="H108" t="inlineStr">
         <is>
-          <t>1485.6884</t>
+          <t>2.7816</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>22.5~23.0</t>
+          <t/>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>-1.96073</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>-1.75589</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>-1.96073</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>-1.6858175</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>-1.95863</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>-1.849505</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H109" t="inlineStr">
-        <is>
-          <t>0.10912502</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="D110" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="E110" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F110" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G110" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="H110" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>

</xml_diff>

<commit_message>
add interface for hompage and cross analysis
</commit_message>
<xml_diff>
--- a/PlantAnalysis/result30210.xlsx
+++ b/PlantAnalysis/result30210.xlsx
@@ -140,32 +140,32 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>3.46816</t>
+          <t>5.90453</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2.3167598</t>
+          <t>2.267735</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>3.4968402</t>
+          <t>3.6348147</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2.75929</t>
+          <t>2.78039</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>3.05431</t>
+          <t>3.12216</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0.2950201</t>
+          <t>0.34176993</t>
         </is>
       </c>
     </row>
@@ -182,32 +182,32 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>3.71883</t>
+          <t>4.71718</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2.77497</t>
+          <t>2.7530904</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>3.7529697</t>
+          <t>3.8002095</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>3.14172</t>
+          <t>3.14576</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>3.38622</t>
+          <t>3.4075398</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>0.24449992</t>
+          <t>0.2617798</t>
         </is>
       </c>
     </row>
@@ -219,37 +219,37 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>3.23279</t>
+          <t>3.153</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>4.03014</t>
+          <t>5.60875</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>3.1867611</t>
+          <t>3.182971</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>4.085471</t>
+          <t>4.0904217</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>3.5237775</t>
+          <t>3.523265</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>3.748455</t>
+          <t>3.7501276</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>0.22467756</t>
+          <t>0.22686267</t>
         </is>
       </c>
     </row>
@@ -266,32 +266,32 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>4.35584</t>
+          <t>7.83407</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>3.62782</t>
+          <t>3.616305</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>4.3972597</t>
+          <t>4.416665</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>3.91636</t>
+          <t>3.91644</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>4.10872</t>
+          <t>4.11653</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>0.19235992</t>
+          <t>0.20008993</t>
         </is>
       </c>
     </row>
@@ -308,32 +308,32 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>4.78218</t>
+          <t>5.31829</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>3.8917284</t>
+          <t>3.8897142</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>4.7945986</t>
+          <t>4.802396</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>4.2303047</t>
+          <t>4.23197</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>4.4560223</t>
+          <t>4.46014</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>0.22571754</t>
+          <t>0.2281704</t>
         </is>
       </c>
     </row>
@@ -345,37 +345,37 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>4.20298</t>
+          <t>3.98932</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>4.91426</t>
+          <t>6.85805</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>4.1754317</t>
+          <t>4.156376</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>4.9193015</t>
+          <t>4.949175</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>4.454383</t>
+          <t>4.4536753</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>4.6403503</t>
+          <t>4.651875</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>0.18596745</t>
+          <t>0.19819975</t>
         </is>
       </c>
     </row>
@@ -387,37 +387,37 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>4.41224</t>
+          <t>4.38959</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>5.12772</t>
+          <t>18.0598</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>4.321109</t>
+          <t>4.3178077</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>5.2120314</t>
+          <t>5.2188277</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>4.655205</t>
+          <t>4.65569</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>4.8779354</t>
+          <t>4.880945</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>0.22273064</t>
+          <t>0.22525501</t>
         </is>
       </c>
     </row>
@@ -434,32 +434,32 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>5.38515</t>
+          <t>5.44308</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>4.5760746</t>
+          <t>4.5721593</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>5.3925953</t>
+          <t>5.3995404</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>4.88227</t>
+          <t>4.882427</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>5.0864</t>
+          <t>5.0892725</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>0.20413017</t>
+          <t>0.20684528</t>
         </is>
       </c>
     </row>
@@ -471,37 +471,37 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>4.95018</t>
+          <t>4.79327</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>5.45509</t>
+          <t>5.76013</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>4.8851676</t>
+          <t>4.8411355</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>5.530088</t>
+          <t>5.5973344</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>5.1270127</t>
+          <t>5.12471</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>5.288243</t>
+          <t>5.31376</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>0.16123009</t>
+          <t>0.18904972</t>
         </is>
       </c>
     </row>
@@ -513,22 +513,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>5.05881</t>
+          <t>4.96568</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>5.73699</t>
+          <t>13.4014</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>4.951241</t>
+          <t>4.929289</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>5.7920117</t>
+          <t>5.828598</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -538,12 +538,12 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>5.4767227</t>
+          <t>5.4913573</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>0.21019268</t>
+          <t>0.22482729</t>
         </is>
       </c>
     </row>
@@ -555,37 +555,37 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>5.13802</t>
+          <t>5.03852</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>5.85495</t>
+          <t>15.6168</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>5.109502</t>
+          <t>5.100115</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>5.8925753</t>
+          <t>5.907755</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>5.4031544</t>
+          <t>5.40298</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>5.5989227</t>
+          <t>5.60489</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>0.19576836</t>
+          <t>0.20191002</t>
         </is>
       </c>
     </row>
@@ -602,32 +602,32 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>5.9321</t>
+          <t>6.07823</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>5.275916</t>
+          <t>5.2747545</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>5.944646</t>
+          <t>5.961623</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>5.52669</t>
+          <t>5.53233</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>5.6938725</t>
+          <t>5.704047</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>0.16718245</t>
+          <t>0.17171717</t>
         </is>
       </c>
     </row>
@@ -644,32 +644,32 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>6.25737</t>
+          <t>6.31977</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>5.3244247</t>
+          <t>5.325613</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>6.308386</t>
+          <t>6.3175125</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>5.69341</t>
+          <t>5.697575</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>5.9394</t>
+          <t>5.94555</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>0.24599028</t>
+          <t>0.24797487</t>
         </is>
       </c>
     </row>
@@ -723,22 +723,22 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>5.7483</t>
+          <t>5.67417</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>6.39308</t>
+          <t>6.77122</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>5.696583</t>
+          <t>5.6832104</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>6.4042225</t>
+          <t>6.42651</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -748,12 +748,12 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>6.1388574</t>
+          <t>6.1477723</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>0.17690992</t>
+          <t>0.18582487</t>
         </is>
       </c>
     </row>
@@ -812,32 +812,32 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>6.61804</t>
+          <t>6.82468</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>5.89896</t>
+          <t>5.8752403</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>6.6757603</t>
+          <t>6.7165203</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>6.19026</t>
+          <t>6.19072</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>6.38446</t>
+          <t>6.40104</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>0.19420004</t>
+          <t>0.21032</t>
         </is>
       </c>
     </row>
@@ -849,37 +849,37 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>6.10651</t>
+          <t>6.05282</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>6.73278</t>
+          <t>6.80508</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>6.071066</t>
+          <t>6.0485573</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>6.743269</t>
+          <t>6.774418</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>6.323142</t>
+          <t>6.320755</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>6.491193</t>
+          <t>6.50222</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>0.16805077</t>
+          <t>0.18146515</t>
         </is>
       </c>
     </row>
@@ -891,37 +891,37 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>6.31666</t>
+          <t>6.22043</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>6.78438</t>
+          <t>6.90125</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>6.237776</t>
+          <t>6.234114</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>6.794134</t>
+          <t>6.7976556</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>6.44641</t>
+          <t>6.445442</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>6.5855</t>
+          <t>6.5863276</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>0.13908958</t>
+          <t>0.14088535</t>
         </is>
       </c>
     </row>
@@ -933,37 +933,37 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>6.39952</t>
+          <t>6.37786</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>6.82628</t>
+          <t>7.01402</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>6.389537</t>
+          <t>6.3819876</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>6.828418</t>
+          <t>6.8431273</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>6.554117</t>
+          <t>6.554915</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>6.6638374</t>
+          <t>6.6702</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>0.10972023</t>
+          <t>0.11528492</t>
         </is>
       </c>
     </row>
@@ -1064,32 +1064,32 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>7.27854</t>
+          <t>8.31837</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>6.581704</t>
+          <t>6.540347</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>7.341893</t>
+          <t>7.416856</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>6.866775</t>
+          <t>6.8690376</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>7.0568223</t>
+          <t>7.088165</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>0.19004726</t>
+          <t>0.21912718</t>
         </is>
       </c>
     </row>
@@ -1106,32 +1106,32 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>7.44421</t>
+          <t>7.53845</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>6.6208544</t>
+          <t>6.5992546</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>7.4869833</t>
+          <t>7.5284557</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>6.9456525</t>
+          <t>6.947705</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>7.1621847</t>
+          <t>7.180005</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>0.21653223</t>
+          <t>0.23230028</t>
         </is>
       </c>
     </row>
@@ -1148,32 +1148,32 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>7.49063</t>
+          <t>7.70039</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>6.7360973</t>
+          <t>6.724562</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>7.639717</t>
+          <t>7.6601624</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>7.074955</t>
+          <t>7.0754123</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>7.30086</t>
+          <t>7.3093123</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>0.22590494</t>
+          <t>0.23390007</t>
         </is>
       </c>
     </row>
@@ -1190,32 +1190,32 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>7.71829</t>
+          <t>7.78158</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>6.699946</t>
+          <t>6.712636</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>7.855864</t>
+          <t>7.8524656</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>7.133415</t>
+          <t>7.1400723</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>7.4223948</t>
+          <t>7.4250298</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>0.28897953</t>
+          <t>0.2849574</t>
         </is>
       </c>
     </row>
@@ -1232,32 +1232,32 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>7.77535</t>
+          <t>7.96707</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>6.9847307</t>
+          <t>6.966036</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>7.8039293</t>
+          <t>7.856634</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>7.29193</t>
+          <t>7.30001</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>7.49673</t>
+          <t>7.52266</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>0.20479965</t>
+          <t>0.22264957</t>
         </is>
       </c>
     </row>
@@ -1358,32 +1358,32 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>8.16639</t>
+          <t>8.27029</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>7.26668</t>
+          <t>7.2707577</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>8.19236</t>
+          <t>8.214697</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>7.61381</t>
+          <t>7.624735</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>7.84523</t>
+          <t>7.8607197</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>0.23142004</t>
+          <t>0.2359848</t>
         </is>
       </c>
     </row>
@@ -1400,32 +1400,32 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>8.17683</t>
+          <t>8.57931</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>7.357216</t>
+          <t>7.3445315</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>8.299665</t>
+          <t>8.330833</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>7.7106347</t>
+          <t>7.7143946</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>7.946247</t>
+          <t>7.96097</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>0.23561239</t>
+          <t>0.24657536</t>
         </is>
       </c>
     </row>
@@ -1442,32 +1442,32 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>8.48147</t>
+          <t>8.61153</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>7.136442</t>
+          <t>7.101737</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>8.74687</t>
+          <t>8.805198</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>7.7403526</t>
+          <t>7.740535</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>8.14296</t>
+          <t>8.1664</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>0.40260696</t>
+          <t>0.42586517</t>
         </is>
       </c>
     </row>
@@ -1484,32 +1484,32 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>8.64726</t>
+          <t>9.86694</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>7.3051987</t>
+          <t>7.301531</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>8.711922</t>
+          <t>8.718462</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>7.83272</t>
+          <t>7.83288</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>8.184401</t>
+          <t>8.187113</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>0.35168076</t>
+          <t>0.3542328</t>
         </is>
       </c>
     </row>
@@ -1526,32 +1526,32 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>8.80308</t>
+          <t>9.06517</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>7.5488973</t>
+          <t>7.5481515</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>8.814373</t>
+          <t>8.817549</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>8.023451</t>
+          <t>8.024176</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>8.33982</t>
+          <t>8.341525</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>0.31636906</t>
+          <t>0.31734943</t>
         </is>
       </c>
     </row>
@@ -1568,32 +1568,32 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>9.05567</t>
+          <t>9.49452</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>7.500131</t>
+          <t>7.506108</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>9.085409</t>
+          <t>9.088699</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>8.09461</t>
+          <t>8.09958</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>8.49093</t>
+          <t>8.495228</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>0.3963194</t>
+          <t>0.395648</t>
         </is>
       </c>
     </row>
@@ -1610,32 +1610,32 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>9.05569</t>
+          <t>9.17856</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>7.6779304</t>
+          <t>7.639133</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>9.068918</t>
+          <t>9.164993</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>8.199551</t>
+          <t>8.21133</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>8.5472975</t>
+          <t>8.592795</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>0.34774685</t>
+          <t>0.38146496</t>
         </is>
       </c>
     </row>
@@ -1694,32 +1694,32 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>9.42961</t>
+          <t>9.70772</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>7.78509</t>
+          <t>7.731089</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>9.43685</t>
+          <t>9.52709</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>8.4045</t>
+          <t>8.40459</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>8.81744</t>
+          <t>8.85359</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>0.41294003</t>
+          <t>0.44900036</t>
         </is>
       </c>
     </row>
@@ -1736,32 +1736,32 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>9.50515</t>
+          <t>9.67238</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>7.840236</t>
+          <t>7.8467073</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>9.529839</t>
+          <t>9.535207</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>8.473837</t>
+          <t>8.479895</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>8.896237</t>
+          <t>8.9020195</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>0.42240047</t>
+          <t>0.42212486</t>
         </is>
       </c>
     </row>
@@ -1820,32 +1820,32 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>9.95315</t>
+          <t>10.3811</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>7.8910246</t>
+          <t>7.892184</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>10.234546</t>
+          <t>10.237844</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>8.769845</t>
+          <t>8.771807</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>9.355725</t>
+          <t>9.358222</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>0.5858803</t>
+          <t>0.5864153</t>
         </is>
       </c>
     </row>
@@ -1862,32 +1862,32 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>10.1859</t>
+          <t>11.0958</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>7.894397</t>
+          <t>7.8758073</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>10.188579</t>
+          <t>10.246187</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>8.754715</t>
+          <t>8.7647</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>9.32826</t>
+          <t>9.357295</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>0.57354546</t>
+          <t>0.5925951</t>
         </is>
       </c>
     </row>
@@ -1904,32 +1904,32 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>10.4996</t>
+          <t>10.7903</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>7.824564</t>
+          <t>7.829176</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>10.699015</t>
+          <t>10.736235</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>8.902483</t>
+          <t>8.919323</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>9.621096</t>
+          <t>9.646088</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>0.7186127</t>
+          <t>0.7267647</t>
         </is>
       </c>
     </row>
@@ -1946,32 +1946,32 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>10.2293</t>
+          <t>10.7492</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>8.282532</t>
+          <t>8.270774</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>10.257992</t>
+          <t>10.343696</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>9.02333</t>
+          <t>9.04812</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>9.517195</t>
+          <t>9.56635</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>0.493865</t>
+          <t>0.51823044</t>
         </is>
       </c>
     </row>
@@ -1988,32 +1988,32 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>10.8424</t>
+          <t>11.1554</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>7.892858</t>
+          <t>7.7534485</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>10.868998</t>
+          <t>11.128067</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>9.00891</t>
+          <t>9.01893</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>9.752945</t>
+          <t>9.862585</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>0.74403477</t>
+          <t>0.84365463</t>
         </is>
       </c>
     </row>
@@ -2030,32 +2030,32 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>11.0772</t>
+          <t>12.5301</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>8.071751</t>
+          <t>7.845324</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>10.9339905</t>
+          <t>11.348646</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>9.14509</t>
+          <t>9.15907</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>9.86065</t>
+          <t>10.034901</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>0.71555996</t>
+          <t>0.87583065</t>
         </is>
       </c>
     </row>
@@ -2072,32 +2072,32 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>11.9792</t>
+          <t>12.1081</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>7.8120813</t>
+          <t>7.8111253</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>11.987031</t>
+          <t>11.992525</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>9.377687</t>
+          <t>9.37915</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>10.421425</t>
+          <t>10.4245</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>1.0437374</t>
+          <t>1.0453501</t>
         </is>
       </c>
     </row>
@@ -2156,32 +2156,32 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>12.6986</t>
+          <t>12.7567</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>7.5930495</t>
+          <t>7.575724</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>12.727972</t>
+          <t>12.747686</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>9.518645</t>
+          <t>9.51521</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>10.802376</t>
+          <t>10.808201</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>1.2837305</t>
+          <t>1.2929907</t>
         </is>
       </c>
     </row>
@@ -2198,32 +2198,32 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>12.8377</t>
+          <t>13.5848</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>7.987313</t>
+          <t>7.850758</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>12.789532</t>
+          <t>13.111305</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>9.788145</t>
+          <t>9.823463</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>10.9887</t>
+          <t>11.1386</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>1.2005548</t>
+          <t>1.3151369</t>
         </is>
       </c>
     </row>
@@ -2245,27 +2245,27 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>7.1573997</t>
+          <t>7.109164</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>14.344881</t>
+          <t>14.440341</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>9.852705</t>
+          <t>9.8583555</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>11.649575</t>
+          <t>11.69115</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>1.7968702</t>
+          <t>1.8327942</t>
         </is>
       </c>
     </row>
@@ -2366,32 +2366,32 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>16.3535</t>
+          <t>20.4419</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>6.908149</t>
+          <t>6.820513</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>17.670952</t>
+          <t>17.829012</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>10.9442</t>
+          <t>10.9487</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>13.6349</t>
+          <t>13.700825</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>2.6907005</t>
+          <t>2.7521248</t>
         </is>
       </c>
     </row>
@@ -2576,32 +2576,32 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>21.9361</t>
+          <t>22.8139</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>6.202902</t>
+          <t>6.2006235</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>22.143698</t>
+          <t>22.178825</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>12.1807</t>
+          <t>12.19245</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>16.1659</t>
+          <t>16.187</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>3.985199</t>
+          <t>3.9945507</t>
         </is>
       </c>
     </row>
@@ -2618,32 +2618,32 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>20.9462</t>
+          <t>21.4889</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>7.3567</t>
+          <t>7.358987</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>22.3559</t>
+          <t>22.377686</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>12.9814</t>
+          <t>12.990999</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>16.7312</t>
+          <t>16.745674</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>3.7497997</t>
+          <t>3.754675</t>
         </is>
       </c>
     </row>
@@ -2744,7 +2744,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>-1.46988</t>
+          <t>-1.2715</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2754,22 +2754,22 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>-1.44486</t>
+          <t>-1.4358326</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>-1.79421</t>
+          <t>-1.789045</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>-1.65447</t>
+          <t>-1.64776</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>0.13973999</t>
+          <t>0.14128494</t>
         </is>
       </c>
     </row>
@@ -2786,7 +2786,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>-1.40992</t>
+          <t>-1.29548</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2796,22 +2796,22 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>-1.3761761</t>
+          <t>-1.3816851</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>-1.85927</t>
+          <t>-1.85471</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>-1.6660324</t>
+          <t>-1.6655</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>0.19323754</t>
+          <t>0.18920994</t>
         </is>
       </c>
     </row>
@@ -2828,7 +2828,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>-1.30932</t>
+          <t>-1.29467</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2838,22 +2838,22 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>-1.30691</t>
+          <t>-1.301195</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>-1.95001</t>
+          <t>-1.946795</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>-1.69277</t>
+          <t>-1.688555</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>0.25723994</t>
+          <t>0.25823998</t>
         </is>
       </c>
     </row>
@@ -2912,7 +2912,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>0.17956</t>
+          <t>4.30075</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2922,22 +2922,22 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>0.4066676</t>
+          <t>0.39910972</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>-3.1500576</t>
+          <t>-3.141965</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>-1.7273675</t>
+          <t>-1.725535</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>1.42269</t>
+          <t>1.4164299</t>
         </is>
       </c>
     </row>
@@ -2954,7 +2954,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>30.949</t>
+          <t>35.4507</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2964,22 +2964,22 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>31.285885</t>
+          <t>31.811443</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>-2.9640076</t>
+          <t>-2.956505</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>10.7359495</t>
+          <t>10.950675</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>13.699957</t>
+          <t>13.90718</t>
         </is>
       </c>
     </row>
@@ -3048,22 +3048,22 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>108.70552</t>
+          <t>108.46505</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>56.0224</t>
+          <t>55.92</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>77.09565</t>
+          <t>76.93802</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>21.07325</t>
+          <t>21.01802</t>
         </is>
       </c>
     </row>
@@ -3080,7 +3080,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>157.922</t>
+          <t>172.664</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -3090,22 +3090,22 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>158.9335</t>
+          <t>159.15579</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>94.2635</t>
+          <t>94.15365</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>120.1315</t>
+          <t>120.1545</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>25.868004</t>
+          <t>26.000854</t>
         </is>
       </c>
     </row>
@@ -3122,7 +3122,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>200.541</t>
+          <t>227.89</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -3132,22 +3132,22 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>226.44897</t>
+          <t>226.55997</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>138.634</t>
+          <t>138.67625</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>173.76</t>
+          <t>173.82974</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>35.12599</t>
+          <t>35.15349</t>
         </is>
       </c>
     </row>
@@ -3216,22 +3216,22 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>422.32397</t>
+          <t>422.666</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>276.22275</t>
+          <t>275.946</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>334.66324</t>
+          <t>334.634</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>58.44049</t>
+          <t>58.68799</t>
         </is>
       </c>
     </row>
@@ -3258,22 +3258,22 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>520.7577</t>
+          <t>523.29755</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>373.52698</t>
+          <t>373.53</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>432.41925</t>
+          <t>433.437</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>58.892273</t>
+          <t>59.907013</t>
         </is>
       </c>
     </row>
@@ -3285,7 +3285,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>418.671</t>
+          <t>403.663</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3295,27 +3295,27 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>418.671</t>
+          <t>403.663</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>641.00275</t>
+          <t>641.1086</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>488.11526</t>
+          <t>487.801</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>549.27026</t>
+          <t>549.124</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>61.155</t>
+          <t>61.32303</t>
         </is>
       </c>
     </row>
@@ -3342,22 +3342,22 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>785.21136</t>
+          <t>783.0171</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>598.1795</t>
+          <t>597.9523</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>672.99225</t>
+          <t>671.9782</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>74.812744</t>
+          <t>74.02594</t>
         </is>
       </c>
     </row>
@@ -3369,7 +3369,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>647.135</t>
+          <t>625.211</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3379,27 +3379,27 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>647.135</t>
+          <t>625.211</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>898.16455</t>
+          <t>899.1222</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>719.282</t>
+          <t>718.38477</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>790.835</t>
+          <t>790.67975</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>71.55304</t>
+          <t>72.29498</t>
         </is>
       </c>
     </row>
@@ -3453,37 +3453,37 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>801.249</t>
+          <t>797.514</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>1209.25</t>
+          <t>1215.23</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>801.249</t>
+          <t>797.514</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>1214.074</t>
+          <t>1215.104</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>935.5465</t>
+          <t>935.25146</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>1046.9575</t>
+          <t>1047.1925</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>111.41101</t>
+          <t>111.94104</t>
         </is>
       </c>
     </row>
@@ -3510,22 +3510,22 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>1378.575</t>
+          <t>1379.3622</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>1024.65</t>
+          <t>1023.66254</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>1166.22</t>
+          <t>1165.9424</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>141.56995</t>
+          <t>142.27985</t>
         </is>
       </c>
     </row>
@@ -3579,7 +3579,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>1032.17</t>
+          <t>1007.6</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3589,27 +3589,27 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>1032.17</t>
+          <t>1007.6</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>1534.135</t>
+          <t>1538.5452</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>1198.21</t>
+          <t>1194.32</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>1332.58</t>
+          <t>1332.01</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>134.37</t>
+          <t>137.69006</t>
         </is>
       </c>
     </row>
@@ -3621,7 +3621,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>1109.16</t>
+          <t>1069.15</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3631,27 +3631,27 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>1109.16</t>
+          <t>1069.15</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>1617.5625</t>
+          <t>1617.7036</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>1244.7626</t>
+          <t>1244.1101</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>1393.8826</t>
+          <t>1393.5475</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>149.12</t>
+          <t>149.43738</t>
         </is>
       </c>
     </row>
@@ -3663,7 +3663,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>1150.08</t>
+          <t>1117.9</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3673,27 +3673,27 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>1150.08</t>
+          <t>1117.9</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>1620.1001</t>
+          <t>1628.7802</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>1292.1</t>
+          <t>1285.48</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>1423.3</t>
+          <t>1422.8</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>131.20007</t>
+          <t>137.32007</t>
         </is>
       </c>
     </row>
@@ -3804,22 +3804,22 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>1664.251</t>
+          <t>1669.0847</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>1341.195</t>
+          <t>1337.81</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>1470.4174</t>
+          <t>1470.32</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>129.22241</t>
+          <t>132.50989</t>
         </is>
       </c>
     </row>
@@ -3831,7 +3831,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>1261.55</t>
+          <t>1227.8</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3841,27 +3841,27 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>1261.55</t>
+          <t>1227.8</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>1641.1511</t>
+          <t>1643.4213</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>1350.2576</t>
+          <t>1346.99</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>1466.615</t>
+          <t>1465.5625</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>116.35742</t>
+          <t>118.57251</t>
         </is>
       </c>
     </row>
@@ -4419,7 +4419,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>1466.42</t>
+          <t>1457.56</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -4429,27 +4429,27 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>1466.42</t>
+          <t>1457.56</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>1512.7101</t>
+          <t>1520.2686</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>1492.01</t>
+          <t>1486.8125</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>1500.29</t>
+          <t>1500.195</t>
         </is>
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>8.280029</t>
+          <t>13.382446</t>
         </is>
       </c>
     </row>
@@ -4508,7 +4508,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>-1.83502</t>
+          <t>1479.62</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -4518,22 +4518,22 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>1.9949852</t>
+          <t>2.2251487</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>-4.59669</t>
+          <t>-4.5938826</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>-1.96002</t>
+          <t>-1.86627</t>
         </is>
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>2.63667</t>
+          <t>2.7276125</t>
         </is>
       </c>
     </row>

</xml_diff>